<commit_message>
inclusão de dois requisitos no plano de ação
</commit_message>
<xml_diff>
--- a/Documentos/PlanoDeAcao.xlsx
+++ b/Documentos/PlanoDeAcao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1327c28a9523567/Documentos/ColdTech/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{72369173-8095-4DBD-A502-E3F9439458D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26CC3157-FA03-4AD1-8585-26B50E2BECC9}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{72369173-8095-4DBD-A502-E3F9439458D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9D728FB-C26A-4C17-8100-6867B27A6DEF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -231,10 +231,25 @@
     <t>Site estátido dashboard</t>
   </si>
   <si>
-    <t>todos da equipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criar da dashboard e linkar junto ao login </t>
+    <t>Todos da equipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criação da dashboard e linkar junto ao login </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagrama de solução </t>
+  </si>
+  <si>
+    <t>Terminar a criação do diagrama de solução</t>
+  </si>
+  <si>
+    <t>slides da apresentação</t>
+  </si>
+  <si>
+    <t>Todos  da equipe</t>
+  </si>
+  <si>
+    <t>Fazer os slides para a apresentação</t>
   </si>
 </sst>
 </file>
@@ -622,6 +637,9 @@
     <xf numFmtId="164" fontId="17" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -645,9 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -697,6 +712,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,8 +1047,8 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1046,24 +1065,24 @@
   <sheetData>
     <row r="1" spans="1:16" ht="45" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:16" s="6" customFormat="1" ht="22.2" customHeight="1">
       <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="38"/>
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
@@ -1081,14 +1100,14 @@
       <c r="B3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="50"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1716,7 +1735,7 @@
       <c r="D40" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="50">
+      <c r="E40" s="42">
         <v>0.3</v>
       </c>
       <c r="F40" s="32">
@@ -1730,22 +1749,50 @@
       </c>
     </row>
     <row r="41" spans="2:8" ht="33" customHeight="1">
-      <c r="B41" s="26"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="26"/>
+      <c r="B41" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="42">
+        <v>0.4</v>
+      </c>
+      <c r="F41" s="32">
+        <v>45219</v>
+      </c>
+      <c r="G41" s="32">
+        <v>45222</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="42" spans="2:8" ht="36.6" customHeight="1">
-      <c r="B42" s="18"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="18"/>
+      <c r="B42" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="36">
+        <v>0</v>
+      </c>
+      <c r="F42" s="19">
+        <v>45219</v>
+      </c>
+      <c r="G42" s="19">
+        <v>45222</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="43" spans="2:8" ht="34.799999999999997" customHeight="1">
       <c r="B43" s="26"/>

</xml_diff>